<commit_message>
implementado relatorio de pendencia
</commit_message>
<xml_diff>
--- a/ControladorGRD/Resources/GRD.xlsx
+++ b/ControladorGRD/Resources/GRD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linco\Documentos\Visual Studio 2019\Repositorio\ControladorGRD\ControladorGRD\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F5C734-B083-4F64-AEA9-45B9D0B16DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B59C5-CCAA-4E78-A08D-EDD454D7AC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2550" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Descrição</t>
   </si>
@@ -226,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -475,6 +475,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -482,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,9 +539,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -551,12 +557,25 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -611,61 +630,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -683,8 +654,59 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1028,7 +1050,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F9" sqref="F9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,62 +1070,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="30" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="33"/>
     </row>
     <row r="2" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="33"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="35"/>
     </row>
     <row r="3" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="33"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="35"/>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1115,25 +1137,25 @@
       <c r="M4" s="8"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" s="29" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="69" t="s">
+    <row r="5" spans="1:14" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="71" t="s">
+      <c r="B5" s="56"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="68"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="54"/>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
@@ -1142,608 +1164,610 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="35"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="38"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="40"/>
     </row>
     <row r="8" spans="1:14" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="19" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48" t="s">
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="49"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="51"/>
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="60"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="63"/>
     </row>
     <row r="10" spans="1:14" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="60"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
     </row>
     <row r="11" spans="1:14" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="60"/>
+      <c r="A11" s="74"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
+      <c r="N11" s="63"/>
     </row>
     <row r="12" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="60"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="63"/>
     </row>
     <row r="13" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="63"/>
     </row>
     <row r="14" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="60"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="63"/>
     </row>
     <row r="15" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="63"/>
     </row>
     <row r="16" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="60"/>
+      <c r="A16" s="74"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="63"/>
     </row>
     <row r="17" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
+      <c r="A17" s="74"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="63"/>
     </row>
     <row r="18" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="60"/>
+      <c r="A18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="63"/>
     </row>
     <row r="19" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
+      <c r="A19" s="74"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="63"/>
     </row>
     <row r="20" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="60"/>
+      <c r="A20" s="74"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="63"/>
     </row>
     <row r="21" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="60"/>
+      <c r="A21" s="74"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="63"/>
     </row>
     <row r="22" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="60"/>
+      <c r="A22" s="74"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="63"/>
     </row>
     <row r="23" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="60"/>
+      <c r="A23" s="74"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="63"/>
     </row>
     <row r="24" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="51"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="60"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="63"/>
     </row>
     <row r="25" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="51"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="60"/>
+      <c r="A25" s="74"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="63"/>
     </row>
     <row r="26" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="60"/>
+      <c r="A26" s="74"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="63"/>
     </row>
     <row r="27" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="60"/>
+      <c r="A27" s="74"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="63"/>
     </row>
     <row r="28" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="51"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="60"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="63"/>
     </row>
     <row r="29" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="60"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="63"/>
     </row>
     <row r="30" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="59"/>
-      <c r="N30" s="60"/>
+      <c r="A30" s="74"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="62"/>
+      <c r="N30" s="63"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="9"/>
-      <c r="C31" s="24"/>
+      <c r="C31" s="23"/>
       <c r="D31" s="9"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="58"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="61"/>
     </row>
     <row r="32" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="57"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="57"/>
-      <c r="N32" s="58"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="61"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="56"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="58"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="61"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="57"/>
-      <c r="K34" s="57"/>
-      <c r="L34" s="57"/>
-      <c r="M34" s="57"/>
-      <c r="N34" s="58"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="61"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="57"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="57"/>
-      <c r="M35" s="57"/>
-      <c r="N35" s="58"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="61"/>
     </row>
     <row r="36" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="65" t="s">
+      <c r="A36" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="66"/>
-      <c r="C36" s="64" t="s">
+      <c r="B36" s="69"/>
+      <c r="C36" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="61" t="s">
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="61"/>
-      <c r="J36" s="61"/>
-      <c r="K36" s="61"/>
-      <c r="L36" s="61"/>
-      <c r="M36" s="61"/>
-      <c r="N36" s="62"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="64"/>
+      <c r="N36" s="65"/>
     </row>
     <row r="37" spans="1:14" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
+      <c r="A37" s="59"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="63" t="s">
+      <c r="F37" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="63"/>
-      <c r="K37" s="63"/>
-      <c r="L37" s="63"/>
-      <c r="M37" s="63"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="66"/>
       <c r="N37" s="18"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
+      <c r="A38" s="59"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="57"/>
-      <c r="M38" s="57"/>
-      <c r="N38" s="58"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="61"/>
+    </row>
+    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="22"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="29"/>
+    </row>
+    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="22"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="29"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="22"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="21"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="22"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="21"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
@@ -1762,30 +1786,29 @@
       <c r="N43" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="97">
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="K17:N17"/>
+  <mergeCells count="102">
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="K29:N29"/>
     <mergeCell ref="K30:N30"/>
     <mergeCell ref="K22:N22"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="F23:J23"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A30:D30"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="K25:N25"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="F26:J26"/>
     <mergeCell ref="K26:N26"/>
+    <mergeCell ref="F30:J30"/>
     <mergeCell ref="K38:N38"/>
     <mergeCell ref="K34:N34"/>
     <mergeCell ref="A35:D35"/>
@@ -1800,6 +1823,12 @@
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="F38:J38"/>
     <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="K10:N10"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="F14:J14"/>
     <mergeCell ref="A11:D11"/>
@@ -1812,12 +1841,6 @@
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="F13:J13"/>
     <mergeCell ref="K13:N13"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="K10:N10"/>
     <mergeCell ref="K33:N33"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="F15:J15"/>
@@ -1834,22 +1857,18 @@
     <mergeCell ref="F28:J28"/>
     <mergeCell ref="K28:N28"/>
     <mergeCell ref="A29:D29"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="C32:J32"/>
     <mergeCell ref="K31:N31"/>
-    <mergeCell ref="F32:J32"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="F30:J30"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="F31:J31"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="K39:N40"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:L5"/>
     <mergeCell ref="E1:N3"/>
     <mergeCell ref="G6:N6"/>
     <mergeCell ref="A7:N7"/>
@@ -1860,6 +1879,16 @@
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:I5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="F33:J33"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="F31:J31"/>
+    <mergeCell ref="F24:J24"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adaptado para sql server
</commit_message>
<xml_diff>
--- a/ControladorGRD/Resources/GRD.xlsx
+++ b/ControladorGRD/Resources/GRD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linco\Documentos\Visual Studio 2019\Repositorio\ControladorGRD\ControladorGRD\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B59C5-CCAA-4E78-A08D-EDD454D7AC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD05607F-1CFC-4A7B-A04D-46490D3EF847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2550" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>GRD:</t>
   </si>
   <si>
-    <t>______________________________________________________</t>
-  </si>
-  <si>
     <t>ASSINATURA DO RECEPTOR</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   <si>
     <t xml:space="preserve"> Observação:</t>
   </si>
+  <si>
+    <t>------------------------------------------------------------------</t>
+  </si>
 </sst>
 </file>
 
@@ -87,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +216,13 @@
       <sz val="26"/>
       <color theme="1"/>
       <name val="PF Square Sans Pro"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Amasis MT Pro Black"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -226,7 +233,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -429,47 +436,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -491,7 +461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -562,6 +532,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -579,7 +552,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -654,9 +627,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,47 +645,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1050,7 +1029,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:J9"/>
+      <selection activeCell="F18" sqref="F18:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,62 +1049,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="32" t="s">
+      <c r="A1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
     </row>
     <row r="2" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="36"/>
     </row>
     <row r="3" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="35"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="36"/>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
       <c r="B4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1138,24 +1117,24 @@
       <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" s="25" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="57" t="s">
+      <c r="A5" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="54"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="55"/>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
@@ -1164,406 +1143,406 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="38"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="40"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" spans="1:14" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50" t="s">
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="52"/>
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="22"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="63"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
     </row>
     <row r="10" spans="1:14" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="74"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+      <c r="N10" s="75"/>
     </row>
     <row r="11" spans="1:14" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="74"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="63"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="75"/>
     </row>
     <row r="12" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="74"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="73"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="63"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="75"/>
     </row>
     <row r="13" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="74"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="63"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="75"/>
     </row>
     <row r="14" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="62"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="63"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="65"/>
+      <c r="N14" s="75"/>
     </row>
     <row r="15" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="74"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="63"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="75"/>
     </row>
     <row r="16" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="73"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="63"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="75"/>
     </row>
     <row r="17" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="74"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="72"/>
-      <c r="I17" s="72"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="63"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="65"/>
+      <c r="L17" s="65"/>
+      <c r="M17" s="65"/>
+      <c r="N17" s="75"/>
     </row>
     <row r="18" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="62"/>
-      <c r="M18" s="62"/>
-      <c r="N18" s="63"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+      <c r="N18" s="75"/>
     </row>
     <row r="19" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="74"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="63"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="65"/>
+      <c r="N19" s="75"/>
     </row>
     <row r="20" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="74"/>
-      <c r="B20" s="75"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="63"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="75"/>
     </row>
     <row r="21" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="74"/>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="62"/>
-      <c r="N21" s="63"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="75"/>
     </row>
     <row r="22" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="74"/>
-      <c r="B22" s="75"/>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="62"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="62"/>
-      <c r="N22" s="63"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+      <c r="N22" s="75"/>
     </row>
     <row r="23" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="74"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="63"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="75"/>
     </row>
     <row r="24" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="74"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="62"/>
-      <c r="N24" s="63"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
+      <c r="M24" s="65"/>
+      <c r="N24" s="75"/>
     </row>
     <row r="25" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="74"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
-      <c r="M25" s="62"/>
-      <c r="N25" s="63"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="75"/>
     </row>
     <row r="26" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="74"/>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="62"/>
-      <c r="N26" s="63"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="75"/>
     </row>
     <row r="27" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="74"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="63"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="75"/>
     </row>
     <row r="28" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="74"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="62"/>
-      <c r="N28" s="63"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="75"/>
     </row>
     <row r="29" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="74"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="62"/>
-      <c r="N29" s="63"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="65"/>
+      <c r="N29" s="75"/>
     </row>
     <row r="30" spans="1:14" s="4" customFormat="1" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="74"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="63"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="75"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
@@ -1571,137 +1550,137 @@
       <c r="C31" s="23"/>
       <c r="D31" s="9"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="61"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="64"/>
     </row>
     <row r="32" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="64"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="62"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="64"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="62"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="64"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="62"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="64"/>
+    </row>
+    <row r="36" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="73"/>
+      <c r="C36" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="71"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="61"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="61"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="61"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="60"/>
-      <c r="L35" s="60"/>
-      <c r="M35" s="60"/>
-      <c r="N35" s="61"/>
-    </row>
-    <row r="36" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="68" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="69"/>
-      <c r="C36" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="64" t="s">
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="77"/>
+    </row>
+    <row r="37" spans="1:14" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="62"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="64"/>
-      <c r="N36" s="65"/>
-    </row>
-    <row r="37" spans="1:14" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="66"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="70"/>
       <c r="N37" s="18"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
-      <c r="B38" s="60"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
+      <c r="A38" s="62"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="61"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="63"/>
+      <c r="K38" s="63"/>
+      <c r="L38" s="63"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="64"/>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
@@ -1713,13 +1692,13 @@
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
       <c r="I39" s="19"/>
-      <c r="J39" s="27" t="s">
+      <c r="J39" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="30"/>
     </row>
     <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
@@ -1731,11 +1710,11 @@
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
       <c r="I40" s="19"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="29"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="30"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>

</xml_diff>